<commit_message>
zweiter doppelter  NRI run
</commit_message>
<xml_diff>
--- a/Durchläufe/NRI/Doppelte NRI/Nachbearbeitung_23_03_02_20_24.xlsx
+++ b/Durchläufe/NRI/Doppelte NRI/Nachbearbeitung_23_03_02_20_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Schell\Documents\GitHub\Limits-to-Growth-Masterprojekt-TH-Koeln-2022\Durchläufe\NRI\Doppelte NRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF120BCF-6399-43B2-AEAC-1FCC125CDA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00637FB2-B947-4E55-BC1C-25AEF9D48EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1648,16 +1648,16 @@
                   <c:v>0.3512003279999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23129100000000002</c:v>
+                  <c:v>-0.23129100000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6000000000000057E-2</c:v>
+                  <c:v>-5.6000000000000057E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.3399999999999923E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69418500000000005</c:v>
+                  <c:v>-0.69418500000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.91178490000000001</c:v>
@@ -1675,10 +1675,10 @@
                   <c:v>0.69198345000000006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.21224758333333327</c:v>
+                  <c:v>-0.21224758333333327</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.34882529008979457</c:v>
+                  <c:v>-0.34882529008979457</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.3177457050309625</c:v>
@@ -1693,16 +1693,16 @@
                   <c:v>4.8191868499999995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.33084734999999998</c:v>
+                  <c:v>-0.33084734999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.13642857142857157</c:v>
+                  <c:v>-0.13642857142857157</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.6052295652173885E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.94668759999999996</c:v>
+                  <c:v>-0.94668759999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7907,7 +7907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE2E520-FB4E-4767-8374-544DD063C850}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -8318,8 +8318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2558A1-7CCA-4408-B812-5A9F3CB1D254}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8371,7 +8371,7 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <f>ABS(C2-D2)/D2</f>
+        <f>(C2-D2)/D2</f>
         <v>6.6215289999999998</v>
       </c>
       <c r="G2" t="s">
@@ -8396,7 +8396,7 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E22" si="0">ABS(C3-D3)/D3</f>
+        <f t="shared" ref="E3:E22" si="0">(C3-D3)/D3</f>
         <v>0.3512003279999999</v>
       </c>
       <c r="G3" t="s">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.23129100000000002</v>
+        <v>-0.23129100000000002</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -8447,7 +8447,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>5.6000000000000057E-2</v>
+        <v>-5.6000000000000057E-2</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -8497,7 +8497,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.69418500000000005</v>
+        <v>-0.69418500000000005</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
@@ -8647,7 +8647,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.21224758333333327</v>
+        <v>-0.21224758333333327</v>
       </c>
       <c r="G13" t="s">
         <v>50</v>
@@ -8672,7 +8672,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0.34882529008979457</v>
+        <v>-0.34882529008979457</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -8779,7 +8779,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0.33084734999999998</v>
+        <v>-0.33084734999999998</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0.13642857142857157</v>
+        <v>-0.13642857142857157</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -8836,7 +8836,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>0.94668759999999996</v>
+        <v>-0.94668759999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>